<commit_message>
fixed a mistake: I was using log10 instead of natural logarithms for the weights
</commit_message>
<xml_diff>
--- a/from_sites_to_matrices/solutions_exo1_fake_matrix.xlsx
+++ b/from_sites_to_matrices/solutions_exo1_fake_matrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="23460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -293,11 +293,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="90">
+  <cellStyleXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -462,7 +484,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="90">
+  <cellStyles count="112">
     <cellStyle name="Lien hypertexte" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="8" builtinId="8" hidden="1"/>
@@ -506,6 +528,17 @@
     <cellStyle name="Lien hypertexte" xfId="84" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="86" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="110" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="9" builtinId="9" hidden="1"/>
@@ -549,6 +582,17 @@
     <cellStyle name="Lien hypertexte visité" xfId="85" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="87" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="111" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Titre 1" xfId="1" builtinId="16"/>
     <cellStyle name="Titre 2" xfId="2" builtinId="17"/>
@@ -948,8 +992,8 @@
   <dimension ref="A1:AM52"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N36" sqref="N36"/>
+      <pane ySplit="7" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L50" sqref="L50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1441,7 +1485,7 @@
         <v>14</v>
       </c>
       <c r="L28" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U28" s="24" t="s">
         <v>14</v>
@@ -1607,19 +1651,19 @@
       </c>
       <c r="L30" s="6">
         <f t="shared" ref="L30:S33" si="15">(B20+$L$28/4)/(B$24+$L$28)</f>
-        <v>0.85</v>
+        <v>0.75</v>
       </c>
       <c r="M30" s="6">
         <f t="shared" si="15"/>
-        <v>0.65</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="N30" s="6">
         <f t="shared" si="15"/>
-        <v>0.45</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="O30" s="6">
         <f t="shared" si="15"/>
-        <v>0.45</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="P30" s="6">
         <f t="shared" si="15"/>
@@ -1627,15 +1671,15 @@
       </c>
       <c r="Q30" s="6">
         <f t="shared" si="15"/>
-        <v>0.05</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="R30" s="6">
         <f t="shared" si="15"/>
-        <v>0.05</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="S30" s="6">
         <f t="shared" si="15"/>
-        <v>0.05</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="U30" s="10" t="s">
         <v>9</v>
@@ -1749,19 +1793,19 @@
       </c>
       <c r="L31" s="7">
         <f t="shared" si="15"/>
-        <v>0.05</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="M31" s="7">
         <f t="shared" si="15"/>
-        <v>0.05</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="N31" s="7">
         <f t="shared" si="15"/>
-        <v>0.05</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="O31" s="7">
         <f t="shared" si="15"/>
-        <v>0.05</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="P31" s="7">
         <f t="shared" si="15"/>
@@ -1769,7 +1813,7 @@
       </c>
       <c r="Q31" s="7">
         <f t="shared" si="15"/>
-        <v>0.45</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="R31" s="7">
         <f t="shared" si="15"/>
@@ -1777,7 +1821,7 @@
       </c>
       <c r="S31" s="7">
         <f t="shared" si="15"/>
-        <v>0.05</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="U31" s="11" t="s">
         <v>10</v>
@@ -1891,15 +1935,15 @@
       </c>
       <c r="L32" s="7">
         <f t="shared" si="15"/>
-        <v>0.05</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="M32" s="7">
         <f t="shared" si="15"/>
-        <v>0.05</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="N32" s="7">
         <f t="shared" si="15"/>
-        <v>0.05</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="O32" s="7">
         <f t="shared" si="15"/>
@@ -1911,15 +1955,15 @@
       </c>
       <c r="Q32" s="7">
         <f t="shared" si="15"/>
-        <v>0.45</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="R32" s="7">
         <f t="shared" si="15"/>
-        <v>0.65</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="S32" s="7">
         <f t="shared" si="15"/>
-        <v>0.85</v>
+        <v>0.75</v>
       </c>
       <c r="U32" s="11" t="s">
         <v>11</v>
@@ -2033,7 +2077,7 @@
       </c>
       <c r="L33" s="8">
         <f t="shared" si="15"/>
-        <v>0.05</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="M33" s="8">
         <f t="shared" si="15"/>
@@ -2041,7 +2085,7 @@
       </c>
       <c r="N33" s="8">
         <f t="shared" si="15"/>
-        <v>0.45</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="O33" s="8">
         <f t="shared" si="15"/>
@@ -2053,15 +2097,15 @@
       </c>
       <c r="Q33" s="8">
         <f t="shared" si="15"/>
-        <v>0.05</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="R33" s="8">
         <f t="shared" si="15"/>
-        <v>0.05</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="S33" s="8">
         <f t="shared" si="15"/>
-        <v>0.05</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="U33" s="12" t="s">
         <v>12</v>
@@ -2304,6 +2348,10 @@
       <c r="B38" s="25">
         <v>0</v>
       </c>
+      <c r="F38" s="22">
+        <f>LN(B30/V40)</f>
+        <v>1.3862943611198906</v>
+      </c>
       <c r="K38" s="24" t="s">
         <v>14</v>
       </c>
@@ -2380,20 +2428,20 @@
         <v>9</v>
       </c>
       <c r="B40" s="18">
-        <f t="shared" ref="B40:I43" si="40">IF(B30=0, "-Inf",LOG(B30/$V40))</f>
-        <v>0.6020599913279624</v>
+        <f>IF(B30=0, "-Inf",LN(B30/$V40))</f>
+        <v>1.3862943611198906</v>
       </c>
       <c r="C40" s="18">
-        <f t="shared" si="40"/>
-        <v>0.47712125471966244</v>
+        <f t="shared" ref="C40:I40" si="40">IF(C30=0, "-Inf",LN(C30/$V40))</f>
+        <v>1.0986122886681098</v>
       </c>
       <c r="D40" s="18">
         <f t="shared" si="40"/>
-        <v>0.3010299956639812</v>
+        <v>0.69314718055994529</v>
       </c>
       <c r="E40" s="18">
         <f t="shared" si="40"/>
-        <v>0.3010299956639812</v>
+        <v>0.69314718055994529</v>
       </c>
       <c r="F40" s="18">
         <f t="shared" si="40"/>
@@ -2415,20 +2463,20 @@
         <v>9</v>
       </c>
       <c r="L40" s="18">
-        <f t="shared" ref="L40:S43" si="41">IF(L30=0, "-Inf",LOG(L30/$V40))</f>
-        <v>0.53147891704225514</v>
+        <f>IF(L30=0, "-Inf",LN(L30/$V40))</f>
+        <v>1.0986122886681098</v>
       </c>
       <c r="M40" s="18">
-        <f t="shared" si="41"/>
-        <v>0.41497334797081797</v>
+        <f t="shared" ref="M40:S40" si="41">IF(M30=0, "-Inf",LN(M30/$V40))</f>
+        <v>0.84729786038720367</v>
       </c>
       <c r="N40" s="18">
         <f t="shared" si="41"/>
-        <v>0.25527250510330607</v>
+        <v>0.51082562376599072</v>
       </c>
       <c r="O40" s="18">
         <f t="shared" si="41"/>
-        <v>0.25527250510330607</v>
+        <v>0.51082562376599072</v>
       </c>
       <c r="P40" s="18">
         <f t="shared" si="41"/>
@@ -2436,15 +2484,15 @@
       </c>
       <c r="Q40" s="18">
         <f t="shared" si="41"/>
-        <v>-0.69897000433601875</v>
+        <v>-1.0986122886681098</v>
       </c>
       <c r="R40" s="18">
         <f t="shared" si="41"/>
-        <v>-0.69897000433601875</v>
+        <v>-1.0986122886681098</v>
       </c>
       <c r="S40" s="18">
         <f t="shared" si="41"/>
-        <v>-0.69897000433601875</v>
+        <v>-1.0986122886681098</v>
       </c>
       <c r="U40" s="6" t="s">
         <v>9</v>
@@ -2458,71 +2506,71 @@
         <v>10</v>
       </c>
       <c r="B41" s="19" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" ref="B41:I41" si="42">IF(B31=0, "-Inf",LN(B31/$V41))</f>
         <v>-Inf</v>
       </c>
       <c r="C41" s="19" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>-Inf</v>
       </c>
       <c r="D41" s="19" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>-Inf</v>
       </c>
       <c r="E41" s="19" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>-Inf</v>
       </c>
       <c r="F41" s="19">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="G41" s="19">
-        <f t="shared" si="40"/>
-        <v>0.3010299956639812</v>
+        <f t="shared" si="42"/>
+        <v>0.69314718055994529</v>
       </c>
       <c r="H41" s="19">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="I41" s="19" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>-Inf</v>
       </c>
       <c r="K41" s="11" t="s">
         <v>10</v>
       </c>
       <c r="L41" s="19">
-        <f t="shared" si="41"/>
-        <v>-0.69897000433601875</v>
+        <f t="shared" ref="L41:S41" si="43">IF(L31=0, "-Inf",LN(L31/$V41))</f>
+        <v>-1.0986122886681098</v>
       </c>
       <c r="M41" s="19">
-        <f t="shared" si="41"/>
-        <v>-0.69897000433601875</v>
+        <f t="shared" si="43"/>
+        <v>-1.0986122886681098</v>
       </c>
       <c r="N41" s="19">
-        <f t="shared" si="41"/>
-        <v>-0.69897000433601875</v>
+        <f t="shared" si="43"/>
+        <v>-1.0986122886681098</v>
       </c>
       <c r="O41" s="19">
-        <f t="shared" si="41"/>
-        <v>-0.69897000433601875</v>
+        <f t="shared" si="43"/>
+        <v>-1.0986122886681098</v>
       </c>
       <c r="P41" s="19">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q41" s="19">
-        <f t="shared" si="41"/>
-        <v>0.25527250510330607</v>
+        <f t="shared" si="43"/>
+        <v>0.51082562376599072</v>
       </c>
       <c r="R41" s="19">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="S41" s="19">
-        <f t="shared" si="41"/>
-        <v>-0.69897000433601875</v>
+        <f t="shared" si="43"/>
+        <v>-1.0986122886681098</v>
       </c>
       <c r="U41" s="7" t="s">
         <v>10</v>
@@ -2536,71 +2584,71 @@
         <v>11</v>
       </c>
       <c r="B42" s="19" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" ref="B42:I42" si="44">IF(B32=0, "-Inf",LN(B32/$V42))</f>
         <v>-Inf</v>
       </c>
       <c r="C42" s="19" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>-Inf</v>
       </c>
       <c r="D42" s="19" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>-Inf</v>
       </c>
       <c r="E42" s="19">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="F42" s="19">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="G42" s="19">
-        <f t="shared" si="40"/>
-        <v>0.3010299956639812</v>
+        <f t="shared" si="44"/>
+        <v>0.69314718055994529</v>
       </c>
       <c r="H42" s="19">
-        <f t="shared" si="40"/>
-        <v>0.47712125471966244</v>
+        <f t="shared" si="44"/>
+        <v>1.0986122886681098</v>
       </c>
       <c r="I42" s="19">
-        <f t="shared" si="40"/>
-        <v>0.6020599913279624</v>
+        <f t="shared" si="44"/>
+        <v>1.3862943611198906</v>
       </c>
       <c r="K42" s="11" t="s">
         <v>11</v>
       </c>
       <c r="L42" s="19">
-        <f t="shared" si="41"/>
-        <v>-0.69897000433601875</v>
+        <f t="shared" ref="L42:S42" si="45">IF(L32=0, "-Inf",LN(L32/$V42))</f>
+        <v>-1.0986122886681098</v>
       </c>
       <c r="M42" s="19">
-        <f t="shared" si="41"/>
-        <v>-0.69897000433601875</v>
+        <f t="shared" si="45"/>
+        <v>-1.0986122886681098</v>
       </c>
       <c r="N42" s="19">
-        <f t="shared" si="41"/>
-        <v>-0.69897000433601875</v>
+        <f t="shared" si="45"/>
+        <v>-1.0986122886681098</v>
       </c>
       <c r="O42" s="19">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="P42" s="19">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="Q42" s="19">
-        <f t="shared" si="41"/>
-        <v>0.25527250510330607</v>
+        <f t="shared" si="45"/>
+        <v>0.51082562376599072</v>
       </c>
       <c r="R42" s="19">
-        <f t="shared" si="41"/>
-        <v>0.41497334797081797</v>
+        <f t="shared" si="45"/>
+        <v>0.84729786038720367</v>
       </c>
       <c r="S42" s="19">
-        <f t="shared" si="41"/>
-        <v>0.53147891704225514</v>
+        <f t="shared" si="45"/>
+        <v>1.0986122886681098</v>
       </c>
       <c r="U42" s="7" t="s">
         <v>11</v>
@@ -2614,71 +2662,71 @@
         <v>12</v>
       </c>
       <c r="B43" s="20" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" ref="B43:I43" si="46">IF(B33=0, "-Inf",LN(B33/$V43))</f>
         <v>-Inf</v>
       </c>
       <c r="C43" s="20">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="D43" s="20">
-        <f t="shared" si="40"/>
-        <v>0.3010299956639812</v>
+        <f t="shared" si="46"/>
+        <v>0.69314718055994529</v>
       </c>
       <c r="E43" s="20">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="F43" s="20">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="G43" s="20" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>-Inf</v>
       </c>
       <c r="H43" s="20" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>-Inf</v>
       </c>
       <c r="I43" s="20" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>-Inf</v>
       </c>
       <c r="K43" s="12" t="s">
         <v>12</v>
       </c>
       <c r="L43" s="20">
-        <f t="shared" si="41"/>
-        <v>-0.69897000433601875</v>
+        <f t="shared" ref="L43:S43" si="47">IF(L33=0, "-Inf",LN(L33/$V43))</f>
+        <v>-1.0986122886681098</v>
       </c>
       <c r="M43" s="20">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="N43" s="20">
-        <f t="shared" si="41"/>
-        <v>0.25527250510330607</v>
+        <f t="shared" si="47"/>
+        <v>0.51082562376599072</v>
       </c>
       <c r="O43" s="20">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="P43" s="20">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="Q43" s="20">
-        <f t="shared" si="41"/>
-        <v>-0.69897000433601875</v>
+        <f t="shared" si="47"/>
+        <v>-1.0986122886681098</v>
       </c>
       <c r="R43" s="20">
-        <f t="shared" si="41"/>
-        <v>-0.69897000433601875</v>
+        <f t="shared" si="47"/>
+        <v>-1.0986122886681098</v>
       </c>
       <c r="S43" s="20">
-        <f t="shared" si="41"/>
-        <v>-0.69897000433601875</v>
+        <f t="shared" si="47"/>
+        <v>-1.0986122886681098</v>
       </c>
       <c r="U43" s="8" t="s">
         <v>12</v>
@@ -2693,70 +2741,70 @@
       </c>
       <c r="B44" s="5">
         <f>SUM(B40:B43)</f>
-        <v>0.6020599913279624</v>
+        <v>1.3862943611198906</v>
       </c>
       <c r="C44" s="5">
-        <f t="shared" ref="C44" si="42">SUM(C40:C43)</f>
-        <v>0.47712125471966244</v>
+        <f t="shared" ref="C44" si="48">SUM(C40:C43)</f>
+        <v>1.0986122886681098</v>
       </c>
       <c r="D44" s="5">
-        <f t="shared" ref="D44" si="43">SUM(D40:D43)</f>
-        <v>0.6020599913279624</v>
+        <f t="shared" ref="D44" si="49">SUM(D40:D43)</f>
+        <v>1.3862943611198906</v>
       </c>
       <c r="E44" s="5">
-        <f t="shared" ref="E44:I44" si="44">SUM(E40:E43)</f>
-        <v>0.3010299956639812</v>
+        <f t="shared" ref="E44:I44" si="50">SUM(E40:E43)</f>
+        <v>0.69314718055994529</v>
       </c>
       <c r="F44" s="5">
-        <f t="shared" ref="F44:H44" si="45">SUM(F40:F43)</f>
+        <f t="shared" ref="F44:H44" si="51">SUM(F40:F43)</f>
         <v>0</v>
       </c>
       <c r="G44" s="5">
-        <f t="shared" si="44"/>
-        <v>0.6020599913279624</v>
+        <f t="shared" si="50"/>
+        <v>1.3862943611198906</v>
       </c>
       <c r="H44" s="5">
-        <f t="shared" si="45"/>
-        <v>0.47712125471966244</v>
+        <f t="shared" si="51"/>
+        <v>1.0986122886681098</v>
       </c>
       <c r="I44" s="5">
-        <f t="shared" si="44"/>
-        <v>0.6020599913279624</v>
+        <f t="shared" si="50"/>
+        <v>1.3862943611198906</v>
       </c>
       <c r="K44" s="13" t="s">
         <v>13</v>
       </c>
       <c r="L44" s="5">
         <f>SUM(L40:L43)</f>
-        <v>-1.5654310959658011</v>
+        <v>-2.1972245773362196</v>
       </c>
       <c r="M44" s="5">
-        <f t="shared" ref="M44" si="46">SUM(M40:M43)</f>
-        <v>-0.98296666070121952</v>
+        <f t="shared" ref="M44" si="52">SUM(M40:M43)</f>
+        <v>-1.3499267169490159</v>
       </c>
       <c r="N44" s="5">
-        <f t="shared" ref="N44" si="47">SUM(N40:N43)</f>
-        <v>-0.88739499846542547</v>
+        <f t="shared" ref="N44" si="53">SUM(N40:N43)</f>
+        <v>-1.1755733298042381</v>
       </c>
       <c r="O44" s="5">
-        <f t="shared" ref="O44:S44" si="48">SUM(O40:O43)</f>
-        <v>-0.44369749923271268</v>
+        <f t="shared" ref="O44:S44" si="54">SUM(O40:O43)</f>
+        <v>-0.58778666490211906</v>
       </c>
       <c r="P44" s="5">
-        <f t="shared" ref="P44:R44" si="49">SUM(P40:P43)</f>
+        <f t="shared" ref="P44:R44" si="55">SUM(P40:P43)</f>
         <v>0</v>
       </c>
       <c r="Q44" s="5">
-        <f t="shared" si="48"/>
-        <v>-0.88739499846542536</v>
+        <f t="shared" si="54"/>
+        <v>-1.1755733298042381</v>
       </c>
       <c r="R44" s="5">
-        <f t="shared" si="49"/>
-        <v>-0.98296666070121952</v>
+        <f t="shared" si="55"/>
+        <v>-1.3499267169490159</v>
       </c>
       <c r="S44" s="5">
-        <f t="shared" si="48"/>
-        <v>-1.5654310959658011</v>
+        <f t="shared" si="54"/>
+        <v>-2.1972245773362196</v>
       </c>
       <c r="U44" s="3"/>
       <c r="V44" s="3"/>
@@ -2850,71 +2898,71 @@
         <v>9</v>
       </c>
       <c r="B48" s="18">
-        <f t="shared" ref="B48:I51" si="50">IF(B30=0, "-Inf",LOG(B30/$V48))</f>
-        <v>0.52287874528033762</v>
+        <f>IF(B30=0, "-Inf",LN(B30/$V48))</f>
+        <v>1.2039728043259361</v>
       </c>
       <c r="C48" s="18">
-        <f t="shared" si="50"/>
-        <v>0.3979400086720376</v>
+        <f t="shared" ref="C48:I48" si="56">IF(C30=0, "-Inf",LN(C30/$V48))</f>
+        <v>0.91629073187415511</v>
       </c>
       <c r="D48" s="18">
-        <f t="shared" si="50"/>
-        <v>0.22184874961635639</v>
+        <f t="shared" si="56"/>
+        <v>0.51082562376599072</v>
       </c>
       <c r="E48" s="18">
-        <f t="shared" si="50"/>
-        <v>0.22184874961635639</v>
+        <f t="shared" si="56"/>
+        <v>0.51082562376599072</v>
       </c>
       <c r="F48" s="18">
-        <f t="shared" si="50"/>
-        <v>-7.9181246047624804E-2</v>
+        <f t="shared" si="56"/>
+        <v>-0.18232155679395459</v>
       </c>
       <c r="G48" s="18" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>-Inf</v>
       </c>
       <c r="H48" s="18" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>-Inf</v>
       </c>
       <c r="I48" s="18" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>-Inf</v>
       </c>
       <c r="K48" s="10" t="s">
         <v>9</v>
       </c>
       <c r="L48" s="18">
-        <f t="shared" ref="L48:S51" si="51">IF(L30=0, "-Inf",LOG(L30/$V48))</f>
-        <v>0.45229767099463031</v>
+        <f>IF(L30=0, "-Inf",LN(L30/$V48))</f>
+        <v>0.91629073187415511</v>
       </c>
       <c r="M48" s="18">
-        <f t="shared" si="51"/>
-        <v>0.3357921019231932</v>
+        <f t="shared" ref="M48:S48" si="57">IF(M30=0, "-Inf",LN(M30/$V48))</f>
+        <v>0.66497630359324911</v>
       </c>
       <c r="N48" s="18">
-        <f t="shared" si="51"/>
-        <v>0.17609125905568124</v>
+        <f t="shared" si="57"/>
+        <v>0.32850406697203616</v>
       </c>
       <c r="O48" s="18">
-        <f t="shared" si="51"/>
-        <v>0.17609125905568124</v>
+        <f t="shared" si="57"/>
+        <v>0.32850406697203616</v>
       </c>
       <c r="P48" s="18">
-        <f t="shared" si="51"/>
-        <v>-7.9181246047624804E-2</v>
+        <f t="shared" si="57"/>
+        <v>-0.18232155679395459</v>
       </c>
       <c r="Q48" s="18">
-        <f t="shared" si="51"/>
-        <v>-0.77815125038364363</v>
+        <f t="shared" si="57"/>
+        <v>-1.2809338454620642</v>
       </c>
       <c r="R48" s="18">
-        <f t="shared" si="51"/>
-        <v>-0.77815125038364363</v>
+        <f t="shared" si="57"/>
+        <v>-1.2809338454620642</v>
       </c>
       <c r="S48" s="18">
-        <f t="shared" si="51"/>
-        <v>-0.77815125038364363</v>
+        <f t="shared" si="57"/>
+        <v>-1.2809338454620642</v>
       </c>
       <c r="U48" s="6" t="s">
         <v>9</v>
@@ -2928,71 +2976,71 @@
         <v>10</v>
       </c>
       <c r="B49" s="19" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" ref="B49:I49" si="58">IF(B31=0, "-Inf",LN(B31/$V49))</f>
         <v>-Inf</v>
       </c>
       <c r="C49" s="19" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="58"/>
         <v>-Inf</v>
       </c>
       <c r="D49" s="19" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="58"/>
         <v>-Inf</v>
       </c>
       <c r="E49" s="19" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="58"/>
         <v>-Inf</v>
       </c>
       <c r="F49" s="19">
-        <f t="shared" si="50"/>
-        <v>9.691001300805642E-2</v>
+        <f t="shared" si="58"/>
+        <v>0.22314355131420976</v>
       </c>
       <c r="G49" s="19">
-        <f t="shared" si="50"/>
-        <v>0.3979400086720376</v>
+        <f t="shared" si="58"/>
+        <v>0.91629073187415511</v>
       </c>
       <c r="H49" s="19">
-        <f t="shared" si="50"/>
-        <v>9.691001300805642E-2</v>
+        <f t="shared" si="58"/>
+        <v>0.22314355131420976</v>
       </c>
       <c r="I49" s="19" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="58"/>
         <v>-Inf</v>
       </c>
       <c r="K49" s="11" t="s">
         <v>10</v>
       </c>
       <c r="L49" s="19">
-        <f t="shared" si="51"/>
-        <v>-0.6020599913279624</v>
+        <f t="shared" ref="L49:S49" si="59">IF(L31=0, "-Inf",LN(L31/$V49))</f>
+        <v>-0.87546873735390007</v>
       </c>
       <c r="M49" s="19">
-        <f t="shared" si="51"/>
-        <v>-0.6020599913279624</v>
+        <f t="shared" si="59"/>
+        <v>-0.87546873735390007</v>
       </c>
       <c r="N49" s="19">
-        <f t="shared" si="51"/>
-        <v>-0.6020599913279624</v>
+        <f t="shared" si="59"/>
+        <v>-0.87546873735390007</v>
       </c>
       <c r="O49" s="19">
-        <f t="shared" si="51"/>
-        <v>-0.6020599913279624</v>
+        <f t="shared" si="59"/>
+        <v>-0.87546873735390007</v>
       </c>
       <c r="P49" s="19">
-        <f t="shared" si="51"/>
-        <v>9.691001300805642E-2</v>
+        <f t="shared" si="59"/>
+        <v>0.22314355131420976</v>
       </c>
       <c r="Q49" s="19">
-        <f t="shared" si="51"/>
-        <v>0.35218251811136247</v>
+        <f t="shared" si="59"/>
+        <v>0.73396917508020054</v>
       </c>
       <c r="R49" s="19">
-        <f t="shared" si="51"/>
-        <v>9.691001300805642E-2</v>
+        <f t="shared" si="59"/>
+        <v>0.22314355131420976</v>
       </c>
       <c r="S49" s="19">
-        <f t="shared" si="51"/>
-        <v>-0.6020599913279624</v>
+        <f t="shared" si="59"/>
+        <v>-0.87546873735390007</v>
       </c>
       <c r="U49" s="7" t="s">
         <v>10</v>
@@ -3006,71 +3054,71 @@
         <v>11</v>
       </c>
       <c r="B50" s="19" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" ref="B50:I50" si="60">IF(B32=0, "-Inf",LN(B32/$V50))</f>
         <v>-Inf</v>
       </c>
       <c r="C50" s="19" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="60"/>
         <v>-Inf</v>
       </c>
       <c r="D50" s="19" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="60"/>
         <v>-Inf</v>
       </c>
       <c r="E50" s="19">
-        <f t="shared" si="50"/>
-        <v>9.691001300805642E-2</v>
+        <f t="shared" si="60"/>
+        <v>0.22314355131420976</v>
       </c>
       <c r="F50" s="19">
-        <f t="shared" si="50"/>
-        <v>9.691001300805642E-2</v>
+        <f t="shared" si="60"/>
+        <v>0.22314355131420976</v>
       </c>
       <c r="G50" s="19">
-        <f t="shared" si="50"/>
-        <v>0.3979400086720376</v>
+        <f t="shared" si="60"/>
+        <v>0.91629073187415511</v>
       </c>
       <c r="H50" s="19">
-        <f t="shared" si="50"/>
-        <v>0.57403126772771884</v>
+        <f t="shared" si="60"/>
+        <v>1.3217558399823195</v>
       </c>
       <c r="I50" s="19">
-        <f t="shared" si="50"/>
-        <v>0.69897000433601886</v>
+        <f t="shared" si="60"/>
+        <v>1.6094379124341003</v>
       </c>
       <c r="K50" s="11" t="s">
         <v>11</v>
       </c>
       <c r="L50" s="19">
-        <f t="shared" si="51"/>
-        <v>-0.6020599913279624</v>
+        <f t="shared" ref="L50:S50" si="61">IF(L32=0, "-Inf",LN(L32/$V50))</f>
+        <v>-0.87546873735390007</v>
       </c>
       <c r="M50" s="19">
-        <f t="shared" si="51"/>
-        <v>-0.6020599913279624</v>
+        <f t="shared" si="61"/>
+        <v>-0.87546873735390007</v>
       </c>
       <c r="N50" s="19">
-        <f t="shared" si="51"/>
-        <v>-0.6020599913279624</v>
+        <f t="shared" si="61"/>
+        <v>-0.87546873735390007</v>
       </c>
       <c r="O50" s="19">
-        <f t="shared" si="51"/>
-        <v>9.691001300805642E-2</v>
+        <f t="shared" si="61"/>
+        <v>0.22314355131420976</v>
       </c>
       <c r="P50" s="19">
-        <f t="shared" si="51"/>
-        <v>9.691001300805642E-2</v>
+        <f t="shared" si="61"/>
+        <v>0.22314355131420976</v>
       </c>
       <c r="Q50" s="19">
-        <f t="shared" si="51"/>
-        <v>0.35218251811136247</v>
+        <f t="shared" si="61"/>
+        <v>0.73396917508020054</v>
       </c>
       <c r="R50" s="19">
-        <f t="shared" si="51"/>
-        <v>0.51188336097887432</v>
+        <f t="shared" si="61"/>
+        <v>1.0704414117014134</v>
       </c>
       <c r="S50" s="19">
-        <f t="shared" si="51"/>
-        <v>0.62838893005031149</v>
+        <f t="shared" si="61"/>
+        <v>1.3217558399823195</v>
       </c>
       <c r="U50" s="7" t="s">
         <v>11</v>
@@ -3084,71 +3132,71 @@
         <v>12</v>
       </c>
       <c r="B51" s="20" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" ref="B51:I51" si="62">IF(B33=0, "-Inf",LN(B33/$V51))</f>
         <v>-Inf</v>
       </c>
       <c r="C51" s="20">
-        <f t="shared" si="50"/>
-        <v>-7.9181246047624804E-2</v>
+        <f t="shared" si="62"/>
+        <v>-0.18232155679395459</v>
       </c>
       <c r="D51" s="20">
-        <f t="shared" si="50"/>
-        <v>0.22184874961635639</v>
+        <f t="shared" si="62"/>
+        <v>0.51082562376599072</v>
       </c>
       <c r="E51" s="20">
-        <f t="shared" si="50"/>
-        <v>-7.9181246047624804E-2</v>
+        <f t="shared" si="62"/>
+        <v>-0.18232155679395459</v>
       </c>
       <c r="F51" s="20">
-        <f t="shared" si="50"/>
-        <v>-7.9181246047624804E-2</v>
+        <f t="shared" si="62"/>
+        <v>-0.18232155679395459</v>
       </c>
       <c r="G51" s="20" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="62"/>
         <v>-Inf</v>
       </c>
       <c r="H51" s="20" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="62"/>
         <v>-Inf</v>
       </c>
       <c r="I51" s="20" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="62"/>
         <v>-Inf</v>
       </c>
       <c r="K51" s="12" t="s">
         <v>12</v>
       </c>
       <c r="L51" s="20">
-        <f t="shared" si="51"/>
-        <v>-0.77815125038364363</v>
+        <f t="shared" ref="L51:S51" si="63">IF(L33=0, "-Inf",LN(L33/$V51))</f>
+        <v>-1.2809338454620642</v>
       </c>
       <c r="M51" s="20">
-        <f t="shared" si="51"/>
-        <v>-7.9181246047624804E-2</v>
+        <f t="shared" si="63"/>
+        <v>-0.18232155679395459</v>
       </c>
       <c r="N51" s="20">
-        <f t="shared" si="51"/>
-        <v>0.17609125905568124</v>
+        <f t="shared" si="63"/>
+        <v>0.32850406697203616</v>
       </c>
       <c r="O51" s="20">
-        <f t="shared" si="51"/>
-        <v>-7.9181246047624804E-2</v>
+        <f t="shared" si="63"/>
+        <v>-0.18232155679395459</v>
       </c>
       <c r="P51" s="20">
-        <f t="shared" si="51"/>
-        <v>-7.9181246047624804E-2</v>
+        <f t="shared" si="63"/>
+        <v>-0.18232155679395459</v>
       </c>
       <c r="Q51" s="20">
-        <f t="shared" si="51"/>
-        <v>-0.77815125038364363</v>
+        <f t="shared" si="63"/>
+        <v>-1.2809338454620642</v>
       </c>
       <c r="R51" s="20">
-        <f t="shared" si="51"/>
-        <v>-0.77815125038364363</v>
+        <f t="shared" si="63"/>
+        <v>-1.2809338454620642</v>
       </c>
       <c r="S51" s="20">
-        <f t="shared" si="51"/>
-        <v>-0.77815125038364363</v>
+        <f t="shared" si="63"/>
+        <v>-1.2809338454620642</v>
       </c>
       <c r="U51" s="8" t="s">
         <v>12</v>
@@ -3163,70 +3211,70 @@
       </c>
       <c r="B52" s="5">
         <f>SUM(B48:B51)</f>
-        <v>0.52287874528033762</v>
+        <v>1.2039728043259361</v>
       </c>
       <c r="C52" s="5">
-        <f t="shared" ref="C52" si="52">SUM(C48:C51)</f>
-        <v>0.31875876262441283</v>
+        <f t="shared" ref="C52" si="64">SUM(C48:C51)</f>
+        <v>0.73396917508020054</v>
       </c>
       <c r="D52" s="5">
-        <f t="shared" ref="D52" si="53">SUM(D48:D51)</f>
-        <v>0.44369749923271279</v>
+        <f t="shared" ref="D52" si="65">SUM(D48:D51)</f>
+        <v>1.0216512475319814</v>
       </c>
       <c r="E52" s="5">
-        <f t="shared" ref="E52:I52" si="54">SUM(E48:E51)</f>
-        <v>0.23957751657678802</v>
+        <f t="shared" ref="E52:I52" si="66">SUM(E48:E51)</f>
+        <v>0.55164761828624587</v>
       </c>
       <c r="F52" s="5">
-        <f t="shared" ref="F52:H52" si="55">SUM(F48:F51)</f>
-        <v>3.5457533920863232E-2</v>
+        <f t="shared" ref="F52:H52" si="67">SUM(F48:F51)</f>
+        <v>8.1643989040510373E-2</v>
       </c>
       <c r="G52" s="5">
-        <f t="shared" si="54"/>
-        <v>0.79588001734407521</v>
+        <f t="shared" si="66"/>
+        <v>1.8325814637483102</v>
       </c>
       <c r="H52" s="5">
-        <f t="shared" si="55"/>
-        <v>0.6709412807357753</v>
+        <f t="shared" si="67"/>
+        <v>1.5448993912965292</v>
       </c>
       <c r="I52" s="5">
-        <f t="shared" si="54"/>
-        <v>0.69897000433601886</v>
+        <f t="shared" si="66"/>
+        <v>1.6094379124341003</v>
       </c>
       <c r="K52" s="13" t="s">
         <v>13</v>
       </c>
       <c r="L52" s="5">
         <f>SUM(L48:L51)</f>
-        <v>-1.5299735620449382</v>
+        <v>-2.1155805882957095</v>
       </c>
       <c r="M52" s="5">
         <f>SUM(M48:M51)</f>
-        <v>-0.94750912678035637</v>
+        <v>-1.2682827279085058</v>
       </c>
       <c r="N52" s="5">
         <f>SUM(N48:N51)</f>
-        <v>-0.85193746454456243</v>
+        <v>-1.0939293407637281</v>
       </c>
       <c r="O52" s="5">
         <f>SUM(O48:O51)</f>
-        <v>-0.40823996531184958</v>
+        <v>-0.50614267586160877</v>
       </c>
       <c r="P52" s="5">
         <f>SUM(P48:P51)</f>
-        <v>3.5457533920863232E-2</v>
+        <v>8.1643989040510373E-2</v>
       </c>
       <c r="Q52" s="5">
-        <f t="shared" ref="Q52:S52" si="56">SUM(Q48:Q51)</f>
-        <v>-0.85193746454456232</v>
+        <f t="shared" ref="Q52:S52" si="68">SUM(Q48:Q51)</f>
+        <v>-1.0939293407637274</v>
       </c>
       <c r="R52" s="5">
-        <f t="shared" si="56"/>
-        <v>-0.94750912678035648</v>
+        <f t="shared" si="68"/>
+        <v>-1.2682827279085054</v>
       </c>
       <c r="S52" s="5">
-        <f t="shared" si="56"/>
-        <v>-1.5299735620449382</v>
+        <f t="shared" si="68"/>
+        <v>-2.1155805882957091</v>
       </c>
       <c r="U52" s="3"/>
       <c r="V52" s="3"/>

</xml_diff>

<commit_message>
added matrices with bg proba for equal and unequal priors
</commit_message>
<xml_diff>
--- a/from_sites_to_matrices/solutions_exo1_fake_matrix.xlsx
+++ b/from_sites_to_matrices/solutions_exo1_fake_matrix.xlsx
@@ -992,8 +992,8 @@
   <dimension ref="A1:AM52"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L50" sqref="L50"/>
+      <pane ySplit="7" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1485,7 +1485,7 @@
         <v>14</v>
       </c>
       <c r="L28" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U28" s="24" t="s">
         <v>14</v>
@@ -1651,19 +1651,19 @@
       </c>
       <c r="L30" s="6">
         <f t="shared" ref="L30:S33" si="15">(B20+$L$28/4)/(B$24+$L$28)</f>
-        <v>0.75</v>
+        <v>0.85</v>
       </c>
       <c r="M30" s="6">
         <f t="shared" si="15"/>
-        <v>0.58333333333333337</v>
+        <v>0.65</v>
       </c>
       <c r="N30" s="6">
         <f t="shared" si="15"/>
-        <v>0.41666666666666669</v>
+        <v>0.45</v>
       </c>
       <c r="O30" s="6">
         <f t="shared" si="15"/>
-        <v>0.41666666666666669</v>
+        <v>0.45</v>
       </c>
       <c r="P30" s="6">
         <f t="shared" si="15"/>
@@ -1671,15 +1671,15 @@
       </c>
       <c r="Q30" s="6">
         <f t="shared" si="15"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.05</v>
       </c>
       <c r="R30" s="6">
         <f t="shared" si="15"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.05</v>
       </c>
       <c r="S30" s="6">
         <f t="shared" si="15"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.05</v>
       </c>
       <c r="U30" s="10" t="s">
         <v>9</v>
@@ -1793,19 +1793,19 @@
       </c>
       <c r="L31" s="7">
         <f t="shared" si="15"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.05</v>
       </c>
       <c r="M31" s="7">
         <f t="shared" si="15"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.05</v>
       </c>
       <c r="N31" s="7">
         <f t="shared" si="15"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.05</v>
       </c>
       <c r="O31" s="7">
         <f t="shared" si="15"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.05</v>
       </c>
       <c r="P31" s="7">
         <f t="shared" si="15"/>
@@ -1813,7 +1813,7 @@
       </c>
       <c r="Q31" s="7">
         <f t="shared" si="15"/>
-        <v>0.41666666666666669</v>
+        <v>0.45</v>
       </c>
       <c r="R31" s="7">
         <f t="shared" si="15"/>
@@ -1821,7 +1821,7 @@
       </c>
       <c r="S31" s="7">
         <f t="shared" si="15"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.05</v>
       </c>
       <c r="U31" s="11" t="s">
         <v>10</v>
@@ -1935,15 +1935,15 @@
       </c>
       <c r="L32" s="7">
         <f t="shared" si="15"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.05</v>
       </c>
       <c r="M32" s="7">
         <f t="shared" si="15"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.05</v>
       </c>
       <c r="N32" s="7">
         <f t="shared" si="15"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.05</v>
       </c>
       <c r="O32" s="7">
         <f t="shared" si="15"/>
@@ -1955,15 +1955,15 @@
       </c>
       <c r="Q32" s="7">
         <f t="shared" si="15"/>
-        <v>0.41666666666666669</v>
+        <v>0.45</v>
       </c>
       <c r="R32" s="7">
         <f t="shared" si="15"/>
-        <v>0.58333333333333337</v>
+        <v>0.65</v>
       </c>
       <c r="S32" s="7">
         <f t="shared" si="15"/>
-        <v>0.75</v>
+        <v>0.85</v>
       </c>
       <c r="U32" s="11" t="s">
         <v>11</v>
@@ -2077,7 +2077,7 @@
       </c>
       <c r="L33" s="8">
         <f t="shared" si="15"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.05</v>
       </c>
       <c r="M33" s="8">
         <f t="shared" si="15"/>
@@ -2085,7 +2085,7 @@
       </c>
       <c r="N33" s="8">
         <f t="shared" si="15"/>
-        <v>0.41666666666666669</v>
+        <v>0.45</v>
       </c>
       <c r="O33" s="8">
         <f t="shared" si="15"/>
@@ -2097,15 +2097,15 @@
       </c>
       <c r="Q33" s="8">
         <f t="shared" si="15"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.05</v>
       </c>
       <c r="R33" s="8">
         <f t="shared" si="15"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.05</v>
       </c>
       <c r="S33" s="8">
         <f t="shared" si="15"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.05</v>
       </c>
       <c r="U33" s="12" t="s">
         <v>12</v>
@@ -2464,19 +2464,19 @@
       </c>
       <c r="L40" s="18">
         <f>IF(L30=0, "-Inf",LN(L30/$V40))</f>
-        <v>1.0986122886681098</v>
+        <v>1.2237754316221157</v>
       </c>
       <c r="M40" s="18">
         <f t="shared" ref="M40:S40" si="41">IF(M30=0, "-Inf",LN(M30/$V40))</f>
-        <v>0.84729786038720367</v>
+        <v>0.95551144502743635</v>
       </c>
       <c r="N40" s="18">
         <f t="shared" si="41"/>
-        <v>0.51082562376599072</v>
+        <v>0.58778666490211906</v>
       </c>
       <c r="O40" s="18">
         <f t="shared" si="41"/>
-        <v>0.51082562376599072</v>
+        <v>0.58778666490211906</v>
       </c>
       <c r="P40" s="18">
         <f t="shared" si="41"/>
@@ -2484,15 +2484,15 @@
       </c>
       <c r="Q40" s="18">
         <f t="shared" si="41"/>
-        <v>-1.0986122886681098</v>
+        <v>-1.6094379124341003</v>
       </c>
       <c r="R40" s="18">
         <f t="shared" si="41"/>
-        <v>-1.0986122886681098</v>
+        <v>-1.6094379124341003</v>
       </c>
       <c r="S40" s="18">
         <f t="shared" si="41"/>
-        <v>-1.0986122886681098</v>
+        <v>-1.6094379124341003</v>
       </c>
       <c r="U40" s="6" t="s">
         <v>9</v>
@@ -2542,19 +2542,19 @@
       </c>
       <c r="L41" s="19">
         <f t="shared" ref="L41:S41" si="43">IF(L31=0, "-Inf",LN(L31/$V41))</f>
-        <v>-1.0986122886681098</v>
+        <v>-1.6094379124341003</v>
       </c>
       <c r="M41" s="19">
         <f t="shared" si="43"/>
-        <v>-1.0986122886681098</v>
+        <v>-1.6094379124341003</v>
       </c>
       <c r="N41" s="19">
         <f t="shared" si="43"/>
-        <v>-1.0986122886681098</v>
+        <v>-1.6094379124341003</v>
       </c>
       <c r="O41" s="19">
         <f t="shared" si="43"/>
-        <v>-1.0986122886681098</v>
+        <v>-1.6094379124341003</v>
       </c>
       <c r="P41" s="19">
         <f t="shared" si="43"/>
@@ -2562,7 +2562,7 @@
       </c>
       <c r="Q41" s="19">
         <f t="shared" si="43"/>
-        <v>0.51082562376599072</v>
+        <v>0.58778666490211906</v>
       </c>
       <c r="R41" s="19">
         <f t="shared" si="43"/>
@@ -2570,7 +2570,7 @@
       </c>
       <c r="S41" s="19">
         <f t="shared" si="43"/>
-        <v>-1.0986122886681098</v>
+        <v>-1.6094379124341003</v>
       </c>
       <c r="U41" s="7" t="s">
         <v>10</v>
@@ -2620,15 +2620,15 @@
       </c>
       <c r="L42" s="19">
         <f t="shared" ref="L42:S42" si="45">IF(L32=0, "-Inf",LN(L32/$V42))</f>
-        <v>-1.0986122886681098</v>
+        <v>-1.6094379124341003</v>
       </c>
       <c r="M42" s="19">
         <f t="shared" si="45"/>
-        <v>-1.0986122886681098</v>
+        <v>-1.6094379124341003</v>
       </c>
       <c r="N42" s="19">
         <f t="shared" si="45"/>
-        <v>-1.0986122886681098</v>
+        <v>-1.6094379124341003</v>
       </c>
       <c r="O42" s="19">
         <f t="shared" si="45"/>
@@ -2640,15 +2640,15 @@
       </c>
       <c r="Q42" s="19">
         <f t="shared" si="45"/>
-        <v>0.51082562376599072</v>
+        <v>0.58778666490211906</v>
       </c>
       <c r="R42" s="19">
         <f t="shared" si="45"/>
-        <v>0.84729786038720367</v>
+        <v>0.95551144502743635</v>
       </c>
       <c r="S42" s="19">
         <f t="shared" si="45"/>
-        <v>1.0986122886681098</v>
+        <v>1.2237754316221157</v>
       </c>
       <c r="U42" s="7" t="s">
         <v>11</v>
@@ -2698,7 +2698,7 @@
       </c>
       <c r="L43" s="20">
         <f t="shared" ref="L43:S43" si="47">IF(L33=0, "-Inf",LN(L33/$V43))</f>
-        <v>-1.0986122886681098</v>
+        <v>-1.6094379124341003</v>
       </c>
       <c r="M43" s="20">
         <f t="shared" si="47"/>
@@ -2706,7 +2706,7 @@
       </c>
       <c r="N43" s="20">
         <f t="shared" si="47"/>
-        <v>0.51082562376599072</v>
+        <v>0.58778666490211906</v>
       </c>
       <c r="O43" s="20">
         <f t="shared" si="47"/>
@@ -2718,15 +2718,15 @@
       </c>
       <c r="Q43" s="20">
         <f t="shared" si="47"/>
-        <v>-1.0986122886681098</v>
+        <v>-1.6094379124341003</v>
       </c>
       <c r="R43" s="20">
         <f t="shared" si="47"/>
-        <v>-1.0986122886681098</v>
+        <v>-1.6094379124341003</v>
       </c>
       <c r="S43" s="20">
         <f t="shared" si="47"/>
-        <v>-1.0986122886681098</v>
+        <v>-1.6094379124341003</v>
       </c>
       <c r="U43" s="8" t="s">
         <v>12</v>
@@ -2776,19 +2776,19 @@
       </c>
       <c r="L44" s="5">
         <f>SUM(L40:L43)</f>
-        <v>-2.1972245773362196</v>
+        <v>-3.604538305680185</v>
       </c>
       <c r="M44" s="5">
         <f t="shared" ref="M44" si="52">SUM(M40:M43)</f>
-        <v>-1.3499267169490159</v>
+        <v>-2.2633643798407643</v>
       </c>
       <c r="N44" s="5">
         <f t="shared" ref="N44" si="53">SUM(N40:N43)</f>
-        <v>-1.1755733298042381</v>
+        <v>-2.0433024950639624</v>
       </c>
       <c r="O44" s="5">
         <f t="shared" ref="O44:S44" si="54">SUM(O40:O43)</f>
-        <v>-0.58778666490211906</v>
+        <v>-1.0216512475319812</v>
       </c>
       <c r="P44" s="5">
         <f t="shared" ref="P44:R44" si="55">SUM(P40:P43)</f>
@@ -2796,15 +2796,15 @@
       </c>
       <c r="Q44" s="5">
         <f t="shared" si="54"/>
-        <v>-1.1755733298042381</v>
+        <v>-2.0433024950639624</v>
       </c>
       <c r="R44" s="5">
         <f t="shared" si="55"/>
-        <v>-1.3499267169490159</v>
+        <v>-2.2633643798407643</v>
       </c>
       <c r="S44" s="5">
         <f t="shared" si="54"/>
-        <v>-2.1972245773362196</v>
+        <v>-3.604538305680185</v>
       </c>
       <c r="U44" s="3"/>
       <c r="V44" s="3"/>
@@ -2934,19 +2934,19 @@
       </c>
       <c r="L48" s="18">
         <f>IF(L30=0, "-Inf",LN(L30/$V48))</f>
-        <v>0.91629073187415511</v>
+        <v>1.0414538748281612</v>
       </c>
       <c r="M48" s="18">
         <f t="shared" ref="M48:S48" si="57">IF(M30=0, "-Inf",LN(M30/$V48))</f>
-        <v>0.66497630359324911</v>
+        <v>0.77318988823348189</v>
       </c>
       <c r="N48" s="18">
         <f t="shared" si="57"/>
-        <v>0.32850406697203616</v>
+        <v>0.40546510810816438</v>
       </c>
       <c r="O48" s="18">
         <f t="shared" si="57"/>
-        <v>0.32850406697203616</v>
+        <v>0.40546510810816438</v>
       </c>
       <c r="P48" s="18">
         <f t="shared" si="57"/>
@@ -2954,15 +2954,15 @@
       </c>
       <c r="Q48" s="18">
         <f t="shared" si="57"/>
-        <v>-1.2809338454620642</v>
+        <v>-1.791759469228055</v>
       </c>
       <c r="R48" s="18">
         <f t="shared" si="57"/>
-        <v>-1.2809338454620642</v>
+        <v>-1.791759469228055</v>
       </c>
       <c r="S48" s="18">
         <f t="shared" si="57"/>
-        <v>-1.2809338454620642</v>
+        <v>-1.791759469228055</v>
       </c>
       <c r="U48" s="6" t="s">
         <v>9</v>
@@ -3012,19 +3012,19 @@
       </c>
       <c r="L49" s="19">
         <f t="shared" ref="L49:S49" si="59">IF(L31=0, "-Inf",LN(L31/$V49))</f>
-        <v>-0.87546873735390007</v>
+        <v>-1.3862943611198906</v>
       </c>
       <c r="M49" s="19">
         <f t="shared" si="59"/>
-        <v>-0.87546873735390007</v>
+        <v>-1.3862943611198906</v>
       </c>
       <c r="N49" s="19">
         <f t="shared" si="59"/>
-        <v>-0.87546873735390007</v>
+        <v>-1.3862943611198906</v>
       </c>
       <c r="O49" s="19">
         <f t="shared" si="59"/>
-        <v>-0.87546873735390007</v>
+        <v>-1.3862943611198906</v>
       </c>
       <c r="P49" s="19">
         <f t="shared" si="59"/>
@@ -3032,7 +3032,7 @@
       </c>
       <c r="Q49" s="19">
         <f t="shared" si="59"/>
-        <v>0.73396917508020054</v>
+        <v>0.81093021621632877</v>
       </c>
       <c r="R49" s="19">
         <f t="shared" si="59"/>
@@ -3040,7 +3040,7 @@
       </c>
       <c r="S49" s="19">
         <f t="shared" si="59"/>
-        <v>-0.87546873735390007</v>
+        <v>-1.3862943611198906</v>
       </c>
       <c r="U49" s="7" t="s">
         <v>10</v>
@@ -3090,15 +3090,15 @@
       </c>
       <c r="L50" s="19">
         <f t="shared" ref="L50:S50" si="61">IF(L32=0, "-Inf",LN(L32/$V50))</f>
-        <v>-0.87546873735390007</v>
+        <v>-1.3862943611198906</v>
       </c>
       <c r="M50" s="19">
         <f t="shared" si="61"/>
-        <v>-0.87546873735390007</v>
+        <v>-1.3862943611198906</v>
       </c>
       <c r="N50" s="19">
         <f t="shared" si="61"/>
-        <v>-0.87546873735390007</v>
+        <v>-1.3862943611198906</v>
       </c>
       <c r="O50" s="19">
         <f t="shared" si="61"/>
@@ -3110,15 +3110,15 @@
       </c>
       <c r="Q50" s="19">
         <f t="shared" si="61"/>
-        <v>0.73396917508020054</v>
+        <v>0.81093021621632877</v>
       </c>
       <c r="R50" s="19">
         <f t="shared" si="61"/>
-        <v>1.0704414117014134</v>
+        <v>1.1786549963416462</v>
       </c>
       <c r="S50" s="19">
         <f t="shared" si="61"/>
-        <v>1.3217558399823195</v>
+        <v>1.4469189829363254</v>
       </c>
       <c r="U50" s="7" t="s">
         <v>11</v>
@@ -3168,7 +3168,7 @@
       </c>
       <c r="L51" s="20">
         <f t="shared" ref="L51:S51" si="63">IF(L33=0, "-Inf",LN(L33/$V51))</f>
-        <v>-1.2809338454620642</v>
+        <v>-1.791759469228055</v>
       </c>
       <c r="M51" s="20">
         <f t="shared" si="63"/>
@@ -3176,7 +3176,7 @@
       </c>
       <c r="N51" s="20">
         <f t="shared" si="63"/>
-        <v>0.32850406697203616</v>
+        <v>0.40546510810816438</v>
       </c>
       <c r="O51" s="20">
         <f t="shared" si="63"/>
@@ -3188,15 +3188,15 @@
       </c>
       <c r="Q51" s="20">
         <f t="shared" si="63"/>
-        <v>-1.2809338454620642</v>
+        <v>-1.791759469228055</v>
       </c>
       <c r="R51" s="20">
         <f t="shared" si="63"/>
-        <v>-1.2809338454620642</v>
+        <v>-1.791759469228055</v>
       </c>
       <c r="S51" s="20">
         <f t="shared" si="63"/>
-        <v>-1.2809338454620642</v>
+        <v>-1.791759469228055</v>
       </c>
       <c r="U51" s="8" t="s">
         <v>12</v>
@@ -3246,19 +3246,19 @@
       </c>
       <c r="L52" s="5">
         <f>SUM(L48:L51)</f>
-        <v>-2.1155805882957095</v>
+        <v>-3.5228943166396749</v>
       </c>
       <c r="M52" s="5">
         <f>SUM(M48:M51)</f>
-        <v>-1.2682827279085058</v>
+        <v>-2.1817203908002538</v>
       </c>
       <c r="N52" s="5">
         <f>SUM(N48:N51)</f>
-        <v>-1.0939293407637281</v>
+        <v>-1.9616585060234526</v>
       </c>
       <c r="O52" s="5">
         <f>SUM(O48:O51)</f>
-        <v>-0.50614267586160877</v>
+        <v>-0.94000725849147104</v>
       </c>
       <c r="P52" s="5">
         <f>SUM(P48:P51)</f>
@@ -3266,15 +3266,15 @@
       </c>
       <c r="Q52" s="5">
         <f t="shared" ref="Q52:S52" si="68">SUM(Q48:Q51)</f>
-        <v>-1.0939293407637274</v>
+        <v>-1.9616585060234524</v>
       </c>
       <c r="R52" s="5">
         <f t="shared" si="68"/>
-        <v>-1.2682827279085054</v>
+        <v>-2.1817203908002538</v>
       </c>
       <c r="S52" s="5">
         <f t="shared" si="68"/>
-        <v>-2.1155805882957091</v>
+        <v>-3.5228943166396749</v>
       </c>
       <c r="U52" s="3"/>
       <c r="V52" s="3"/>

</xml_diff>